<commit_message>
Fixed writing from textTo Excel
</commit_message>
<xml_diff>
--- a/testare.xlsx
+++ b/testare.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>Nume</t>
   </si>
@@ -35,40 +35,85 @@
     <t>IS21Z</t>
   </si>
   <si>
+    <t>DA</t>
+  </si>
+  <si>
+    <t>Turcanu</t>
+  </si>
+  <si>
+    <t>Tudor</t>
+  </si>
+  <si>
     <t>Da</t>
   </si>
   <si>
-    <t>Turcanu</t>
-  </si>
-  <si>
-    <t>Tudor</t>
-  </si>
-  <si>
     <t>Lungu</t>
   </si>
   <si>
     <t>Andrei</t>
   </si>
   <si>
-    <t>Nu</t>
+    <t>Cabac</t>
+  </si>
+  <si>
+    <t>Valeria</t>
+  </si>
+  <si>
+    <t>IS11Z</t>
+  </si>
+  <si>
+    <t>Popov</t>
+  </si>
+  <si>
+    <t>Marinela</t>
+  </si>
+  <si>
+    <t>Dumitru</t>
+  </si>
+  <si>
+    <t>IS21z</t>
   </si>
   <si>
     <t>Bazaochi</t>
   </si>
   <si>
-    <t>Dumitru</t>
-  </si>
-  <si>
-    <t>Popov</t>
-  </si>
-  <si>
-    <t>Marinela</t>
-  </si>
-  <si>
     <t>Eminescu</t>
   </si>
   <si>
     <t>MIhai</t>
+  </si>
+  <si>
+    <t>Anton</t>
+  </si>
+  <si>
+    <t>Carbuneanu</t>
+  </si>
+  <si>
+    <t>da</t>
+  </si>
+  <si>
+    <t>Elizarov</t>
+  </si>
+  <si>
+    <t>Alexei</t>
+  </si>
+  <si>
+    <t>is21z</t>
+  </si>
+  <si>
+    <t>Munteanu</t>
+  </si>
+  <si>
+    <t>Victor</t>
+  </si>
+  <si>
+    <t>Iatco</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>nu</t>
   </si>
 </sst>
 </file>
@@ -113,7 +158,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -158,21 +203,21 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -183,7 +228,7 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -191,10 +236,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -205,13 +250,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -219,16 +264,86 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
To fix writing to Excel File
</commit_message>
<xml_diff>
--- a/testare.xlsx
+++ b/testare.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Nume</t>
   </si>
@@ -27,6 +27,27 @@
   </si>
   <si>
     <t>Media</t>
+  </si>
+  <si>
+    <t>Creanga</t>
+  </si>
+  <si>
+    <t>Ion</t>
+  </si>
+  <si>
+    <t>IS21Z</t>
+  </si>
+  <si>
+    <t>DA</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>Turcanu</t>
+  </si>
+  <si>
+    <t>Turodr</t>
   </si>
 </sst>
 </file>
@@ -71,7 +92,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -94,6 +115,56 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>